<commit_message>
WIP Waterfall rights import updates#9488
</commit_message>
<xml_diff>
--- a/assets/templates/import-documents-template.xlsx
+++ b/assets/templates/import-documents-template.xlsx
@@ -874,12 +874,12 @@
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="A10" activeCellId="0" sqref="10:10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -9457,7 +9457,7 @@
     <mergeCell ref="L110:L120"/>
     <mergeCell ref="M110:M120"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q10:S10" type="none">
       <formula1>languages</formula1>
       <formula2>0</formula2>
@@ -9467,6 +9467,10 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="List of choice - Please select a choice from that list." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B11:B120" type="none">
+      <formula1>#ref!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="List of choice - Please select a choice from that list." showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G10" type="none">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
changed contract type, added expenses, changed payment date and statement status & debug
</commit_message>
<xml_diff>
--- a/assets/templates/import-documents-template.xlsx
+++ b/assets/templates/import-documents-template.xlsx
@@ -158,7 +158,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">//  'mandate' | 'sale'</t>
+      <t xml:space="preserve">//  Rightholder rôle</t>
     </r>
   </si>
   <si>
@@ -272,7 +272,7 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -284,7 +284,7 @@
       <rPr>
         <b val="true"/>
         <sz val="6"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -322,7 +322,7 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -334,7 +334,7 @@
       <rPr>
         <b val="true"/>
         <sz val="6"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -873,13 +873,13 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A10" activeCellId="0" sqref="10:10"/>
+      <selection pane="topRight" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -1145,13 +1145,13 @@
       <c r="M10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="25" t="s">
+      <c r="N10" s="26" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="26" t="s">
         <v>16</v>
       </c>
       <c r="Q10" s="26" t="s">

</xml_diff>

<commit_message>
added rightholder profit graph (#9526)
* added rightholder profit graph

* filtered blocks related to statement on dashboard

* cleaned graph

* added income per source graph

* debug dashboard if not statement

* updated attributes visibility

* statements improvement: use right contractId

* changed contract type, added expenses, changed payment date and statement status & debug

* small debug

---------

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-documents-template.xlsx
+++ b/assets/templates/import-documents-template.xlsx
@@ -158,7 +158,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">//  'mandate' | 'sale'</t>
+      <t xml:space="preserve">//  Rightholder rôle</t>
     </r>
   </si>
   <si>
@@ -272,7 +272,7 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -284,7 +284,7 @@
       <rPr>
         <b val="true"/>
         <sz val="6"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -322,7 +322,7 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -334,7 +334,7 @@
       <rPr>
         <b val="true"/>
         <sz val="6"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -873,13 +873,13 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A10" activeCellId="0" sqref="10:10"/>
+      <selection pane="topRight" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -1145,13 +1145,13 @@
       <c r="M10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="25" t="s">
+      <c r="N10" s="26" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="26" t="s">
         <v>16</v>
       </c>
       <c r="Q10" s="26" t="s">

</xml_diff>

<commit_message>
ok feat #9556 add contract name
</commit_message>
<xml_diff>
--- a/assets/templates/import-documents-template.xlsx
+++ b/assets/templates/import-documents-template.xlsx
@@ -85,24 +85,13 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Document ID
+      <t xml:space="preserve">Document Name
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">// Will be generated automatically if empty</t>
     </r>
   </si>
   <si>
@@ -118,7 +107,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Root ID
+      <t xml:space="preserve">Root Document Name
 </t>
     </r>
     <r>
@@ -130,7 +119,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// If this contract is an amendment, provide root contract Id</t>
+      <t xml:space="preserve">// If this contract is an amendment, provide root contract name</t>
     </r>
   </si>
   <si>
@@ -873,13 +862,13 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N10" activeCellId="0" sqref="N10"/>
+      <selection pane="topRight" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -1112,7 +1101,7 @@
       <c r="B10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="25" t="s">

</xml_diff>

<commit_message>
feat #9556 add contract name (#9558)
* tmp #9556

* ok feat #9556 add contract name

---------

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-documents-template.xlsx
+++ b/assets/templates/import-documents-template.xlsx
@@ -85,24 +85,13 @@
       <rPr>
         <b val="true"/>
         <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Document ID
+      <t xml:space="preserve">Document Name
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">// Will be generated automatically if empty</t>
     </r>
   </si>
   <si>
@@ -118,7 +107,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Root ID
+      <t xml:space="preserve">Root Document Name
 </t>
     </r>
     <r>
@@ -130,7 +119,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// If this contract is an amendment, provide root contract Id</t>
+      <t xml:space="preserve">// If this contract is an amendment, provide root contract name</t>
     </r>
   </si>
   <si>
@@ -873,13 +862,13 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N10" activeCellId="0" sqref="N10"/>
+      <selection pane="topRight" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -1112,7 +1101,7 @@
       <c r="B10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="25" t="s">

</xml_diff>